<commit_message>
Updated plan according to SQA
</commit_message>
<xml_diff>
--- a/dev_11Jun2009/docs/Induction/Induction Plan.xlsx
+++ b/dev_11Jun2009/docs/Induction/Induction Plan.xlsx
@@ -16,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Session</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Domain Induction</t>
-  </si>
-  <si>
-    <t>About the product</t>
-  </si>
-  <si>
     <t>Admin Demo</t>
   </si>
   <si>
@@ -45,18 +36,59 @@
     <t>30 min</t>
   </si>
   <si>
-    <t>Technical Training</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>Areas</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Basic Biology</t>
+  </si>
+  <si>
+    <t>caGrid Induction</t>
+  </si>
+  <si>
+    <t>Product Demo</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>2 hr</t>
+  </si>
+  <si>
+    <t>Overall architechture</t>
+  </si>
+  <si>
+    <t>Introduction to model</t>
+  </si>
+  <si>
+    <t>3 hr</t>
+  </si>
+  <si>
+    <t>Technical Session</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,83 +413,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C9" t="s">
         <v>5</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated according to Sujata's comment
</commit_message>
<xml_diff>
--- a/dev_11Jun2009/docs/Induction/Induction Plan.xlsx
+++ b/dev_11Jun2009/docs/Induction/Induction Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Time</t>
   </si>
@@ -73,6 +73,51 @@
   </si>
   <si>
     <t>Technical Session</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Madhumita Shrikhande</t>
+  </si>
+  <si>
+    <t>Chandrakant Talele</t>
+  </si>
+  <si>
+    <t>Pooja Arora</t>
+  </si>
+  <si>
+    <t>SVN reporistory under docs/Induction</t>
+  </si>
+  <si>
+    <t>Introduction to concepts of biology, like gene, DNA etc</t>
+  </si>
+  <si>
+    <t>Demonstration of all the Admin module features</t>
+  </si>
+  <si>
+    <t>Demonstration of all the web application features</t>
+  </si>
+  <si>
+    <t>Demonstration of all the Desktop Application features</t>
+  </si>
+  <si>
+    <t>User Manual in SVN repository</t>
+  </si>
+  <si>
+    <t>Design and Archtechture Document in SVN repository</t>
+  </si>
+  <si>
+    <t>Concepts about caBIG, their objective, what is caGRID, how the data is stored etc</t>
+  </si>
+  <si>
+    <t>Explanation of the design and overall architechture of the entire application</t>
   </si>
 </sst>
 </file>
@@ -413,18 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -434,8 +481,17 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -445,8 +501,17 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -456,8 +521,14 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -467,8 +538,17 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -478,8 +558,17 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -489,8 +578,17 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -500,8 +598,17 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -511,8 +618,14 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -521,6 +634,9 @@
       </c>
       <c r="C9" t="s">
         <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>